<commit_message>
docs: update the documentation site to represent the new match-ref and segmented arguments both on commandline and and in samplesheet
</commit_message>
<xml_diff>
--- a/docs/samples.xlsx
+++ b/docs/samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\zwagemaf\projects\ViroConstrictor\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\zwagemaf\projects\ViroConstrictor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812B457B-2F54-421A-BC7D-B469E7C86DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0290AD56-A078-42D0-978D-1014C0FCBE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15705" yWindow="-15240" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13575" yWindow="-16440" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Sample</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>/path/to/HPV_reference.fasta</t>
+  </si>
+  <si>
+    <t>Segmented</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,14 +434,15 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" customWidth="1"/>
-    <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,22 +453,25 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -474,23 +481,26 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>50</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -498,25 +508,28 @@
         <v>7</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>30</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -524,25 +537,28 @@
         <v>20</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>30</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -552,19 +568,22 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>